<commit_message>
LoginTestCest (Criação) - Teste Funcional Obrigatorio
O seguinte teste funcional não se encontra a funcionar de momento
</commit_message>
<xml_diff>
--- a/Documentacao/Plano_Testes/Template_PlanoTestes.xlsx
+++ b/Documentacao/Plano_Testes/Template_PlanoTestes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JoanaPedrosa\Documents\AULAS_202021\1Semestre_PLSI\ENUNCIADO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/IPL_PSI_ProjetoFinal_SARAMAGO/Documentacao/Plano_Testes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E892B3-F039-431B-82FC-5515E6203A37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969AFE8E-7D3C-5849-92B3-C964192D9AEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{95683A14-184E-4B3C-BA7D-5CA753ECF9F9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" activeTab="2" xr2:uid="{95683A14-184E-4B3C-BA7D-5CA753ECF9F9}"/>
   </bookViews>
   <sheets>
     <sheet name="PlanoTestes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
   <si>
     <t>Nome do Projeto</t>
   </si>
@@ -100,6 +100,24 @@
   </si>
   <si>
     <t>Plataformas de Sistemas de Informação       |      D + PL      |      2020/21</t>
+  </si>
+  <si>
+    <t>SARAMAGO</t>
+  </si>
+  <si>
+    <t>André Machado</t>
+  </si>
+  <si>
+    <t>Gonçalo Rocha</t>
+  </si>
+  <si>
+    <t>Login (LoginTestCest)</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Backend</t>
   </si>
 </sst>
 </file>
@@ -576,7 +594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -625,12 +643,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -640,73 +689,45 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1023,69 +1044,71 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C581CB-E1F9-4895-AECD-C1EB3A0EDA78}">
   <dimension ref="B2:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26:I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" customWidth="1"/>
-    <col min="2" max="2" width="19.21875" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" customWidth="1"/>
+    <col min="1" max="1" width="5.5" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="45" t="s">
+    <row r="2" spans="2:15" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="40"/>
-    </row>
-    <row r="3" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:15" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="25" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="23"/>
+    </row>
+    <row r="3" spans="2:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="2:15" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="38"/>
-    </row>
-    <row r="5" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="2:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="21"/>
+    </row>
+    <row r="5" spans="2:15" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="43"/>
-      <c r="M6" s="44"/>
-    </row>
-    <row r="7" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C6" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="25"/>
+    </row>
+    <row r="7" spans="2:15" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -1099,218 +1122,230 @@
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="2:15" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="22" t="s">
+    <row r="8" spans="2:15" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:15" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="24"/>
-    </row>
-    <row r="10" spans="2:15" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="35"/>
+    </row>
+    <row r="10" spans="2:15" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="30"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C11" s="1"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="33"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C12" s="1"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="33"/>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C13" s="1"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="33"/>
-      <c r="O13" s="47"/>
-    </row>
-    <row r="16" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="38"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C11" s="1">
+        <v>2180622</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="41"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C12" s="1">
+        <v>2180659</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="41"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C13" s="1">
+        <v>2180</v>
+      </c>
+      <c r="D13" s="39"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="41"/>
+      <c r="O13" s="26"/>
+    </row>
+    <row r="16" spans="2:15" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-    </row>
-    <row r="24" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+    </row>
+    <row r="24" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C26" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" s="9"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -1320,36 +1355,36 @@
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
     </row>
-    <row r="32" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="C33" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -1390,42 +1425,42 @@
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="4" width="8.88671875" customWidth="1"/>
+    <col min="2" max="4" width="8.83203125" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="11.21875" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" customWidth="1"/>
     <col min="10" max="10" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+    <row r="2" spans="2:12" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="27"/>
-    </row>
-    <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="45"/>
+    </row>
+    <row r="5" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
       <c r="I6" s="16" t="s">
         <v>16</v>
       </c>
@@ -1433,68 +1468,68 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
       <c r="I7" s="11"/>
       <c r="J7" s="12"/>
     </row>
-    <row r="8" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
       <c r="I8" s="11"/>
       <c r="J8" s="12"/>
     </row>
-    <row r="9" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
       <c r="I9" s="11"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
       <c r="I10" s="11"/>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
       <c r="I11" s="13"/>
       <c r="J11" s="14"/>
     </row>
@@ -1518,44 +1553,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2388E85-4066-4F58-9827-09010DD3CF52}">
   <dimension ref="B2:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="9" max="9" width="13.33203125" customWidth="1"/>
-    <col min="10" max="10" width="10.44140625" customWidth="1"/>
+    <col min="10" max="10" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="21" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+    <row r="2" spans="2:12" ht="21" x14ac:dyDescent="0.2">
+      <c r="B2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="27"/>
-    </row>
-    <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="2:12" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="45"/>
+    </row>
+    <row r="5" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:12" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
       <c r="I6" s="16" t="s">
         <v>18</v>
       </c>
@@ -1563,68 +1598,72 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="11"/>
+      <c r="C7" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="J7" s="12"/>
     </row>
-    <row r="8" spans="2:12" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
       <c r="I8" s="11"/>
       <c r="J8" s="12"/>
     </row>
-    <row r="9" spans="2:12" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
       <c r="I9" s="11"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="2:12" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
       <c r="I10" s="11"/>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="2:12" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12" ht="25.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
       <c r="I11" s="13"/>
       <c r="J11" s="14"/>
     </row>
@@ -1650,51 +1689,51 @@
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="9" max="9" width="12.77734375" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+    <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.2">
+      <c r="B2" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="27"/>
-    </row>
-    <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="45"/>
+    </row>
+    <row r="4" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
       <c r="I5" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
       <c r="I6" s="14"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização do plano de testes
</commit_message>
<xml_diff>
--- a/Documentacao/Plano_Testes/Template_PlanoTestes.xlsx
+++ b/Documentacao/Plano_Testes/Template_PlanoTestes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/IPL_PSI_ProjetoFinal_SARAMAGO/Documentacao/Plano_Testes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\IPL_PSI_ProjetoFinal2\Documentacao\Plano_Testes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969AFE8E-7D3C-5849-92B3-C964192D9AEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B03535-7AB7-49A9-B115-0FD57BAB0BB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" activeTab="2" xr2:uid="{95683A14-184E-4B3C-BA7D-5CA753ECF9F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{95683A14-184E-4B3C-BA7D-5CA753ECF9F9}"/>
   </bookViews>
   <sheets>
     <sheet name="PlanoTestes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="30">
   <si>
     <t>Nome do Projeto</t>
   </si>
@@ -111,13 +111,22 @@
     <t>Gonçalo Rocha</t>
   </si>
   <si>
-    <t>Login (LoginTestCest)</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
     <t>Backend</t>
+  </si>
+  <si>
+    <t>Criar Leitor</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Criar Leitor(CreateLeitorCest) / Adicionar um leitor através do leitor/create/_form</t>
+  </si>
+  <si>
+    <t>Login (LoginTestCest) / Realizar o login de um admin no backend</t>
   </si>
 </sst>
 </file>
@@ -662,33 +671,30 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -705,6 +711,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1048,49 +1057,49 @@
       <selection activeCell="C26" sqref="C26:I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" customWidth="1"/>
-    <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="31" t="s">
+    <row r="2" spans="2:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
       <c r="L2" s="22"/>
       <c r="M2" s="23"/>
     </row>
-    <row r="3" spans="2:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="2:15" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="29" t="s">
+    <row r="3" spans="2:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:15" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
       <c r="L4" s="20"/>
       <c r="M4" s="21"/>
     </row>
-    <row r="5" spans="2:15" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
@@ -1108,7 +1117,7 @@
       <c r="L6" s="24"/>
       <c r="M6" s="25"/>
     </row>
-    <row r="7" spans="2:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -1122,230 +1131,232 @@
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="2:15" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:15" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="33" t="s">
+    <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="2:15" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="35"/>
-    </row>
-    <row r="10" spans="2:15" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="33"/>
+    </row>
+    <row r="10" spans="2:15" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="38"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="37"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C11" s="1">
         <v>2180622</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="41"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="40"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C12" s="1">
         <v>2180659</v>
       </c>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="41"/>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="40"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C13" s="1">
         <v>2180</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="41"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="40"/>
       <c r="O13" s="26"/>
     </row>
-    <row r="16" spans="2:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27"/>
-    </row>
-    <row r="24" spans="2:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+    </row>
+    <row r="24" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="41"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C26" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C27" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="34"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="9"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -1355,39 +1366,47 @@
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
     </row>
-    <row r="32" spans="2:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C33" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="41"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C33:I33"/>
+    <mergeCell ref="C34:I34"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="C29:I29"/>
     <mergeCell ref="B4:K4"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="C9:I9"/>
@@ -1402,14 +1421,6 @@
     <mergeCell ref="C20:I20"/>
     <mergeCell ref="C21:I21"/>
     <mergeCell ref="C6:K6"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="C33:I33"/>
-    <mergeCell ref="C34:I34"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="C29:I29"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1425,31 +1436,31 @@
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="8.83203125" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" customWidth="1"/>
+    <col min="2" max="4" width="8.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="29" t="s">
+    <row r="2" spans="2:12" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
       <c r="L2" s="45"/>
     </row>
-    <row r="5" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>14</v>
       </c>
@@ -1468,7 +1479,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>9</v>
       </c>
@@ -1481,7 +1492,7 @@
       <c r="I7" s="11"/>
       <c r="J7" s="12"/>
     </row>
-    <row r="8" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>10</v>
       </c>
@@ -1494,7 +1505,7 @@
       <c r="I8" s="11"/>
       <c r="J8" s="12"/>
     </row>
-    <row r="9" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>11</v>
       </c>
@@ -1507,7 +1518,7 @@
       <c r="I9" s="11"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>12</v>
       </c>
@@ -1520,7 +1531,7 @@
       <c r="I10" s="11"/>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>13</v>
       </c>
@@ -1554,32 +1565,32 @@
   <dimension ref="B2:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:H7"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
-    <col min="10" max="10" width="10.5" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="21" x14ac:dyDescent="0.2">
-      <c r="B2" s="29" t="s">
+    <row r="2" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
       <c r="L2" s="45"/>
     </row>
-    <row r="5" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:12" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:12" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>14</v>
       </c>
@@ -1598,12 +1609,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:12" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="48"/>
       <c r="E7" s="48"/>
@@ -1611,24 +1622,32 @@
       <c r="G7" s="48"/>
       <c r="H7" s="48"/>
       <c r="I7" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" s="12"/>
-    </row>
-    <row r="8" spans="2:12" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="12"/>
-    </row>
-    <row r="9" spans="2:12" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>11</v>
       </c>
@@ -1641,7 +1660,7 @@
       <c r="I9" s="11"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="2:12" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:12" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>12</v>
       </c>
@@ -1654,7 +1673,7 @@
       <c r="I10" s="11"/>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="2:12" ht="25.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="25.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>13</v>
       </c>
@@ -1689,26 +1708,26 @@
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.2">
-      <c r="B2" s="29" t="s">
+    <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
       <c r="J2" s="45"/>
     </row>
-    <row r="4" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
         <v>14</v>
       </c>
@@ -1724,7 +1743,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" ht="23.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="19" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
+1 teste funcional, diversos fixes
</commit_message>
<xml_diff>
--- a/Documentacao/Plano_Testes/Template_PlanoTestes.xlsx
+++ b/Documentacao/Plano_Testes/Template_PlanoTestes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\IPL_PSI_ProjetoFinal2\Documentacao\Plano_Testes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B03535-7AB7-49A9-B115-0FD57BAB0BB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF6B5C3-87D8-4CDF-BCF4-A32F252925B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{95683A14-184E-4B3C-BA7D-5CA753ECF9F9}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
   <si>
     <t>Nome do Projeto</t>
   </si>
@@ -111,22 +111,37 @@
     <t>Gonçalo Rocha</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
     <t>Backend</t>
   </si>
   <si>
-    <t>Criar Leitor</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
-    <t>Criar Leitor(CreateLeitorCest) / Adicionar um leitor através do leitor/create/_form</t>
-  </si>
-  <si>
-    <t>Login (LoginTestCest) / Realizar o login de um admin no backend</t>
+    <t>Efetuar Login como admin</t>
+  </si>
+  <si>
+    <t>Criar um leitor como admin</t>
+  </si>
+  <si>
+    <t>Criar leitor com validações corretas</t>
+  </si>
+  <si>
+    <t>Leitor</t>
+  </si>
+  <si>
+    <t>Criar Leitor (CreateLeitorTest) / Criar leitor com validações corretas</t>
+  </si>
+  <si>
+    <t>Login (LoginBackendCest) / Realizar o login de um admin no backend</t>
+  </si>
+  <si>
+    <t>Criar Leitor(CreateLeitorCest) / Adicionar um leitor através do 'leitor/create/_form'</t>
+  </si>
+  <si>
+    <t>CreateBibliotecaCest / Adicionar uma biblioteca através de 'biblioteca/create/_form'</t>
+  </si>
+  <si>
+    <t>Criar uma biblioteca como admin</t>
   </si>
 </sst>
 </file>
@@ -603,7 +618,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -671,6 +686,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -692,9 +716,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -713,9 +734,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -735,6 +753,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1053,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C581CB-E1F9-4895-AECD-C1EB3A0EDA78}">
   <dimension ref="B2:O34"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:I26"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29:I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,35 +1087,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
       <c r="L2" s="22"/>
       <c r="M2" s="23"/>
     </row>
     <row r="3" spans="2:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:15" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
       <c r="L4" s="20"/>
       <c r="M4" s="21"/>
     </row>
@@ -1103,17 +1124,17 @@
       <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
       <c r="L6" s="24"/>
       <c r="M6" s="25"/>
     </row>
@@ -1133,65 +1154,65 @@
     </row>
     <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="2:15" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="33"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="36"/>
     </row>
     <row r="10" spans="2:15" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="37"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="39"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C11" s="1">
         <v>2180622</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="40"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="42"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C12" s="1">
         <v>2180659</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="40"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="42"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C13" s="1">
         <v>2180</v>
       </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="42"/>
       <c r="O13" s="26"/>
     </row>
     <row r="16" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1203,75 +1224,77 @@
       <c r="B17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
+      <c r="C18" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
     </row>
     <row r="24" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
@@ -1282,79 +1305,81 @@
       <c r="B25" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="41" t="s">
+      <c r="C25" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="41"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
+      <c r="C26" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
+      <c r="C27" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
+      <c r="C28" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="34"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="34"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="9"/>
@@ -1375,38 +1400,30 @@
       <c r="B33" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="41" t="s">
+      <c r="C33" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="41"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="34"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="C33:I33"/>
-    <mergeCell ref="C34:I34"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="C29:I29"/>
     <mergeCell ref="B4:K4"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="C9:I9"/>
@@ -1421,6 +1438,14 @@
     <mergeCell ref="C20:I20"/>
     <mergeCell ref="C21:I21"/>
     <mergeCell ref="C6:K6"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C33:I33"/>
+    <mergeCell ref="C34:I34"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="C29:I29"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1433,7 +1458,7 @@
   <dimension ref="B2:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1445,33 +1470,33 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="45"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="46"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
       <c r="I6" s="16" t="s">
         <v>16</v>
       </c>
@@ -1483,25 +1508,31 @@
       <c r="B7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="12"/>
+      <c r="C7" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="50" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
       <c r="I8" s="11"/>
       <c r="J8" s="12"/>
     </row>
@@ -1509,12 +1540,12 @@
       <c r="B9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
       <c r="I9" s="11"/>
       <c r="J9" s="12"/>
     </row>
@@ -1522,12 +1553,12 @@
       <c r="B10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
       <c r="I10" s="11"/>
       <c r="J10" s="12"/>
     </row>
@@ -1535,12 +1566,12 @@
       <c r="B11" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
       <c r="I11" s="13"/>
       <c r="J11" s="14"/>
     </row>
@@ -1565,7 +1596,7 @@
   <dimension ref="B2:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1575,33 +1606,33 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="45"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="46"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:12" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
       <c r="I6" s="16" t="s">
         <v>18</v>
       </c>
@@ -1613,63 +1644,69 @@
       <c r="B7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48"/>
-      <c r="I7" s="11" t="s">
+      <c r="J7" s="50" t="s">
         <v>25</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="11" t="s">
+      <c r="C8" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="50" t="s">
         <v>25</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="12"/>
+      <c r="C9" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="50" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="2:12" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
       <c r="I10" s="11"/>
       <c r="J10" s="12"/>
     </row>
@@ -1677,12 +1714,12 @@
       <c r="B11" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
       <c r="I11" s="13"/>
       <c r="J11" s="14"/>
     </row>
@@ -1714,31 +1751,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="45"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="46"/>
     </row>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
       <c r="I5" s="17" t="s">
         <v>17</v>
       </c>
@@ -1747,12 +1784,12 @@
       <c r="B6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
       <c r="I6" s="14"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Plano de testes update
</commit_message>
<xml_diff>
--- a/Documentacao/Plano_Testes/Template_PlanoTestes.xlsx
+++ b/Documentacao/Plano_Testes/Template_PlanoTestes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\wamp64\www\IPL_PSI_ProjetoFinal2\Documentacao\Plano_Testes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\IPL_PSI_ProjetoFinal2\Documentacao\Plano_Testes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66267984-0F3B-457A-BA8D-7D630469EBBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE653EF9-0E65-46E3-9230-7A796CF5E774}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="9072" xr2:uid="{95683A14-184E-4B3C-BA7D-5CA753ECF9F9}"/>
+    <workbookView xWindow="1950" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{95683A14-184E-4B3C-BA7D-5CA753ECF9F9}"/>
   </bookViews>
   <sheets>
     <sheet name="PlanoTestes" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="53">
   <si>
     <t>Nome do Projeto</t>
   </si>
@@ -180,6 +180,21 @@
   </si>
   <si>
     <t>Criar Biblioteca (CreateBibliotecaTest / Criar biblioteca com validações corretas</t>
+  </si>
+  <si>
+    <t>Criar Tipo de Leitor (CreateTipoLeitorTest) / Criar Tipo de leitor e verificar na BD</t>
+  </si>
+  <si>
+    <t>Associar Leitor (LeitorAssociateCest) / Associar uma role a um leitor</t>
+  </si>
+  <si>
+    <t>Associar uma role nova a um leitor pré-existente</t>
+  </si>
+  <si>
+    <t>Criar um Tipo de Leitor</t>
+  </si>
+  <si>
+    <t>TipoLeitor</t>
   </si>
 </sst>
 </file>
@@ -656,7 +671,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -725,6 +740,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -746,9 +773,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -767,9 +791,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -777,7 +798,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -786,15 +807,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -815,7 +827,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1113,71 +1125,71 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C581CB-E1F9-4895-AECD-C1EB3A0EDA78}">
   <dimension ref="B2:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:I20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="28" t="s">
+    <row r="2" spans="2:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
       <c r="L2" s="18"/>
       <c r="M2" s="19"/>
     </row>
-    <row r="3" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:15" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="26" t="s">
+    <row r="3" spans="2:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:15" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
       <c r="L4" s="16"/>
       <c r="M4" s="17"/>
     </row>
-    <row r="5" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="2:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
       <c r="L6" s="20"/>
       <c r="M6" s="21"/>
     </row>
-    <row r="7" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -1191,244 +1203,248 @@
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="2:15" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="30" t="s">
+    <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="2:15" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="32"/>
-    </row>
-    <row r="10" spans="2:15" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="36"/>
+    </row>
+    <row r="10" spans="2:15" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="36"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="39"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C11" s="1">
         <v>2180622</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="39"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="42"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C12" s="1">
         <v>2180659</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="39"/>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="42"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C13" s="1">
         <v>2180696</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="39"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="42"/>
       <c r="O13" s="22"/>
     </row>
-    <row r="16" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="C20" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C21" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-    </row>
-    <row r="24" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+    </row>
+    <row r="24" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="40" t="s">
+      <c r="C25" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="33" t="s">
+      <c r="C26" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="33" t="s">
+      <c r="C27" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="33" t="s">
+      <c r="C28" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="33" t="s">
+      <c r="C29" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C30" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="9"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -1438,64 +1454,55 @@
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
     </row>
-    <row r="32" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="40" t="s">
+      <c r="C33" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="40"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="40"/>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="33" t="s">
+      <c r="C34" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="28"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="33" t="s">
+      <c r="C35" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="33"/>
-      <c r="I35" s="33"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="C35:I35"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="C33:I33"/>
-    <mergeCell ref="C34:I34"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="C29:I29"/>
     <mergeCell ref="B4:K4"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="C9:I9"/>
@@ -1510,6 +1517,15 @@
     <mergeCell ref="C20:I20"/>
     <mergeCell ref="C21:I21"/>
     <mergeCell ref="C6:K6"/>
+    <mergeCell ref="C35:I35"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C33:I33"/>
+    <mergeCell ref="C34:I34"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="C29:I29"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1522,45 +1538,45 @@
   <dimension ref="B2:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="8.88671875" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" customWidth="1"/>
+    <col min="2" max="4" width="8.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+    <row r="2" spans="2:12" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="44"/>
-    </row>
-    <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="46"/>
+    </row>
+    <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
       <c r="I6" s="12" t="s">
         <v>16</v>
       </c>
@@ -1568,18 +1584,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
       <c r="I7" s="23" t="s">
         <v>29</v>
       </c>
@@ -1587,18 +1603,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
       <c r="I8" s="24" t="s">
         <v>43</v>
       </c>
@@ -1606,18 +1622,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
       <c r="I9" s="24" t="s">
         <v>45</v>
       </c>
@@ -1625,31 +1641,37 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="25"/>
-    </row>
-    <row r="11" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" s="25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="48"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1672,43 +1694,43 @@
   <dimension ref="B2:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:H11"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
-    <col min="10" max="10" width="10.44140625" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="21" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+    <row r="2" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="B2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="44"/>
-    </row>
-    <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="2:12" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="46"/>
+    </row>
+    <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:12" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
       <c r="I6" s="12" t="s">
         <v>18</v>
       </c>
@@ -1716,18 +1738,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
       <c r="I7" s="23" t="s">
         <v>24</v>
       </c>
@@ -1735,18 +1757,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
       <c r="I8" s="23" t="s">
         <v>24</v>
       </c>
@@ -1754,18 +1776,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
       <c r="I9" s="23" t="s">
         <v>24</v>
       </c>
@@ -1773,18 +1795,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
       <c r="I10" s="24" t="s">
         <v>24</v>
       </c>
@@ -1792,18 +1814,24 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="25.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12" ht="25.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="48"/>
+      <c r="C11" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="27" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1827,70 +1855,70 @@
       <selection activeCell="C6" sqref="C6:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="12.88671875" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+    <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="B2" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="44"/>
-    </row>
-    <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="46"/>
+    </row>
+    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
       <c r="I5" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" ht="23.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="48" t="s">
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="48" t="s">
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="27" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>